<commit_message>
test elec sec US files
</commit_message>
<xml_diff>
--- a/InputData/elec/BZECfNP/BAU Zero Emis Credit for Nuc Plants.xlsx
+++ b/InputData/elec/BZECfNP/BAU Zero Emis Credit for Nuc Plants.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\RMI\RMI_all_states\NV\elec\BZECfNP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BZECfNP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D0D0640-DF1F-43D9-8567-96D116BED563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C95D32-173E-43B1-AAF5-49BCDB4B8A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="660" windowWidth="16755" windowHeight="14505" activeTab="1" xr2:uid="{C5EFE8E4-8660-49B5-88C2-8D099D44E411}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C5EFE8E4-8660-49B5-88C2-8D099D44E411}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="BZECfNP" sheetId="2" r:id="rId3"/>
+    <sheet name="BZECfNP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>BZECfNP BAU Zero Emissions Credit for Nuclear Plants</t>
   </si>
@@ -146,313 +145,13 @@
   </si>
   <si>
     <t>hydrogen combined cycle</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>Alaska</t>
-  </si>
-  <si>
-    <t>AK</t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
-    <t>AZ</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>AR</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>Colorado</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
-    <t>CT</t>
-  </si>
-  <si>
-    <t>Delaware</t>
-  </si>
-  <si>
-    <t>DE</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>GA</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>HI</t>
-  </si>
-  <si>
-    <t>Idaho</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>IL</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>Iowa</t>
-  </si>
-  <si>
-    <t>IA</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>KS</t>
-  </si>
-  <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t>KY</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
-  </si>
-  <si>
-    <t>LA</t>
-  </si>
-  <si>
-    <t>Maine</t>
-  </si>
-  <si>
-    <t>ME</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>Massachusetts</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>MI</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>MN</t>
-  </si>
-  <si>
-    <t>Mississippi</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>MO</t>
-  </si>
-  <si>
-    <t>Montana</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>NE</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>NV</t>
-  </si>
-  <si>
-    <t>New Hampshire</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>NJ</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>NM</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>NY</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
-    <t>NC</t>
-  </si>
-  <si>
-    <t>North Dakota</t>
-  </si>
-  <si>
-    <t>ND</t>
-  </si>
-  <si>
-    <t>Ohio</t>
-  </si>
-  <si>
-    <t>OH</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>PA</t>
-  </si>
-  <si>
-    <t>Rhode Island</t>
-  </si>
-  <si>
-    <t>RI</t>
-  </si>
-  <si>
-    <t>South Carolina</t>
-  </si>
-  <si>
-    <t>SC</t>
-  </si>
-  <si>
-    <t>South Dakota</t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>TN</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>TX</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>UT</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>VT</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>VA</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>WA</t>
-  </si>
-  <si>
-    <t>West Virginia</t>
-  </si>
-  <si>
-    <t>WV</t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
-    <t>WI</t>
-  </si>
-  <si>
-    <t>Wyoming</t>
-  </si>
-  <si>
-    <t>WY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,13 +179,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -519,7 +211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -529,8 +221,6 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -846,474 +536,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD24FED-1FE2-4888-B6B4-6A2AD33A9CF5}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="8">
-        <v>45293</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="str">
-        <f>LOOKUP(B1,F1:G50,G1:G50)</f>
-        <v>NV</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2019</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F7" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F11" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F14" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>0.13</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F17" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <f>A13*A16</f>
         <v>1.9500000000000002</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F20" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F21" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F22" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F23" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F24" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F25" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F26" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F27" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F28" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F29" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F30" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F31" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F32" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F33" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F34" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F35" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F36" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F37" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F38" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F39" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F40" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F41" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F42" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F43" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F44" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F45" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F46" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F47" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F48" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F49" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F50" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1325,57 +631,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5219AD4A-B58F-488A-85D3-8AC59C46BE97}">
-  <dimension ref="A2:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E711EE28-FA43-4667-9C9B-C8367E936C88}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:AE25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>